<commit_message>
Atualização de dados 22/01/2024: SKU e CNPJ
</commit_message>
<xml_diff>
--- a/shelflife/cnpj.xlsx
+++ b/shelflife/cnpj.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dato\OneDrive\Documentos\Datoo\repositorio\python\shelflife\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dato\Documents\REPOSITÓRIO\PYTHON\shelflife\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AABD9B19-4F69-44A5-A84A-83B35FB0D596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F320B34-E931-4586-A9D4-7A9FFF02B49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -19,22 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$A$1842</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="1840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="1840">
   <si>
     <t>CPF/CNPJ</t>
   </si>
@@ -5559,7 +5548,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5615,9 +5604,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5655,7 +5644,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5761,7 +5750,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5903,18 +5892,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1842"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A1843"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A1843" sqref="A2:A1843"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15132,8 +15121,13 @@
         <v>1839</v>
       </c>
     </row>
+    <row r="1843" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1843" t="s">
+        <v>1056</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A1842"/>
+  <autoFilter ref="A1:A1842" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>